<commit_message>
toArray added to excelWorkbook
toArray is the only function that will output processed data from the excelWorkbook  object. It is then encoded to JSON by the controller. This allows more flexibility.

The last row can now be found. It does not have great accuracy, but it is working.
</commit_message>
<xml_diff>
--- a/userdata/data_test.xlsx
+++ b/userdata/data_test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -101,6 +101,21 @@
   </si>
   <si>
     <t>other stuff that is actually a comment or something</t>
+  </si>
+  <si>
+    <t>dsa</t>
+  </si>
+  <si>
+    <t>sa</t>
+  </si>
+  <si>
+    <t>ds</t>
+  </si>
+  <si>
+    <t>saf</t>
+  </si>
+  <si>
+    <t>af</t>
   </si>
 </sst>
 </file>
@@ -448,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:I46"/>
+  <dimension ref="A2:Q88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,22 +480,59 @@
     <col min="7" max="7" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
       <c r="G5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -506,7 +558,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
@@ -529,7 +581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -552,7 +604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -574,8 +626,11 @@
       <c r="G11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -598,7 +653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -620,8 +675,11 @@
       <c r="G13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -644,7 +702,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -667,7 +725,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -690,7 +748,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -713,7 +771,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -736,7 +794,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -759,7 +817,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -781,8 +839,14 @@
       <c r="G20">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K20" t="s">
+        <v>25</v>
+      </c>
+      <c r="L20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -805,7 +869,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -827,8 +891,11 @@
       <c r="G22">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -850,8 +917,11 @@
       <c r="G23">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="P23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -874,7 +944,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -897,7 +967,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -920,7 +990,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -943,7 +1013,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -965,8 +1035,14 @@
       <c r="G28">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>30</v>
+      </c>
+      <c r="L28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -989,7 +1065,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1012,7 +1088,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -1034,8 +1110,11 @@
       <c r="G31">
         <v>23</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -1058,7 +1137,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -1080,8 +1159,11 @@
       <c r="G33">
         <v>25</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="O33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -1103,8 +1185,11 @@
       <c r="G34">
         <v>26</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -1126,8 +1211,11 @@
       <c r="G35">
         <v>27</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -1150,7 +1238,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -1173,7 +1261,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>16</v>
       </c>
@@ -1195,8 +1283,16 @@
       <c r="G38">
         <v>30</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>25</v>
       </c>
@@ -1210,14 +1306,91 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>24</v>
+      </c>
       <c r="C46" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>24</v>
+      </c>
+      <c r="J48" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>32</v>
+      </c>
+      <c r="J55" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N59" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>30</v>
+      </c>
+      <c r="F60" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="66" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G66" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="72" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="P72" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="74" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G74" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="83" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="Q83" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="84" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F84" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="88" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="L88" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>